<commit_message>
codigo funcionando... pesquisador de pecas de pc
</commit_message>
<xml_diff>
--- a/computadormontado.xlsx
+++ b/computadormontado.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005054889735.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECLkQ&amp;usg=AOvVaw2IfqQPBazqxB8E8y9rEnnQ</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005054889735.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECJ4Q&amp;usg=AOvVaw1IGz8ZalLbMveSI0Gqzp3m</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005010762271.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECKIU&amp;usg=AOvVaw0YXmXjVGn_n6NUlJaSeVZC</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005010762271.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECOoT&amp;usg=AOvVaw2mg4I8ewgSmO0iSPbKzQLL</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005012530788.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECIIR&amp;usg=AOvVaw1OONjNVBFP5TSU8hKI0kDW</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005012530788.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECNsQ&amp;usg=AOvVaw1jvt3Y8InPBh4R7t374EHB</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004421523541.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECLcP&amp;usg=AOvVaw1ZeX9sTz9Q5KYqDvVC3IDq</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004421523541.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECKsP&amp;usg=AOvVaw1crSwL1l3e_BSrTT0CEGzl</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/365050/placa-mae-msi-pro-h610m-b-ddr4-lga1700-matx-ddr4%3Fsrsltid%3DAd5pg_F9laKwbDVtgMXMJHsgGnvTddAl4NIZ7-_nmWU9xrobhMFEY3yISsE&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECIsP&amp;usg=AOvVaw2LnkFvGVCdkXiLTXqXQzlu</t>
+          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/365050/placa-mae-msi-pro-h610m-b-ddr4-lga1700-matx-ddr4%3Fsrsltid%3DAd5pg_FRAr7Nfw8GMlOWnlaJ8bBQRdc6Swc3jNg89_CbLGgaaUu2yMRTEZ4&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECP8O&amp;usg=AOvVaw0uGfHPL5WNGqPGwl64YaPl</t>
         </is>
       </c>
     </row>
@@ -536,142 +536,142 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004161480649.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECJ8K&amp;usg=AOvVaw3UOUrf05vvwlxoiFsMXI_K</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004161480649.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECLAK&amp;usg=AOvVaw2JwTxmvjgfMM_6yxWMcFWS</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>placa mae mancer h610m-dard, ddr4, socket lga1700, m-atx</t>
+          <t>asus placa-mãe prime h610m-e d4-csm preto</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>529.9</v>
+        <v>524.99</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pichau.com.br/placa-mae-mancer-h610m-dard-ddr4-socket-lga1700-m-atx-chipset-intel-h610-mcr-h610m-dard%3Fsrsltid%3DAd5pg_HSkZ1yu-NXupQ-6ZDXrOWYUzV5Gjfw-CcCcX7oaL3DsA2fTmEmfw0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECMQP&amp;usg=AOvVaw2LGFOK5y5ykxavC9swC-jD</t>
+          <t>https://www.google.com.br/url?url=https://www.tradeinn.com/techinn/pt/asus-placa-mae-prime-h610m-e-d4-csm/138689543/p%3Futm_source%3Dgoogle_products%26utm_medium%3Dmerchant%26id_producte%3D15514226%26country%3Dbr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECKMU&amp;usg=AOvVaw0TGv565zb_-QOV7MWz-dOj</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>nova marca intel i3 12100f desktop gaming cpu oem chip apenas 10th gen ...</t>
+          <t>placa mae mancer h610m-dard, ddr4, socket lga1700, m-atx</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>545.33</v>
+        <v>529.9</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005029573107.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECKkM&amp;usg=AOvVaw2fiwAswWXSES-hbdx_ZN4R</t>
+          <t>https://www.google.com.br/url?url=https://www.pichau.com.br/placa-mae-mancer-h610m-dard-ddr4-socket-lga1700-m-atx-chipset-intel-h610-mcr-h610m-dard%3Fsrsltid%3DAd5pg_H6X4H6sKUxyhF5vfNY_FyADRsSr2D50llPG_GkZMZUykgAeuuUUzs&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECLgP&amp;usg=AOvVaw1AxVXXDCA0b8ol19VDwgnA</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>placa mãe duex dx h610zg m2 (lga 1700/intel h610/m.2)</t>
+          <t>nova marca intel i3 12100f desktop gaming cpu oem chip apenas 10th gen ...</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>549.9</v>
+        <v>545.33</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.terabyteshop.com.br/produto/23732/placa-mae-duex-dx-h610zg-chipset-h610-intel-lga-1700-matx-ddr4%3Fsrsltid%3DAd5pg_EKghu3Wb-gYtQZzdUaeL7KY37Cu-4UuS3reRLVvBmA97W-UKJd64Q&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECOgN&amp;usg=AOvVaw3LDGI3Kc-GsmRtEdN17Lbs</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005029573107.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECLoM&amp;usg=AOvVaw3sPGNSGVd560S_mBrKna67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>núcleo i3-12100f i3 12100f 3.3 ghz 4-core processador cpu de 8 linhas l3 = 12m ...</t>
+          <t>placa mãe duex dx h610zg m2 (lga 1700/intel h610/m.2)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>549.92</v>
+        <v>549.9</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005195505536.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECOAK&amp;usg=AOvVaw2m7298A8Az8Ukm9SvPosqp</t>
+          <t>https://www.google.com.br/url?url=https://www.terabyteshop.com.br/produto/23732/placa-mae-duex-dx-h610zg-chipset-h610-intel-lga-1700-matx-ddr4%3Fsrsltid%3DAd5pg_FxLED_DRQlzfaswr3lLUNzyzeyMC59_JprgNWU9qtA7yh45cOsy1M&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECNwN&amp;usg=AOvVaw0w1YlJlRjogcOzUYNrcweP</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>100% novo intel core i3 12100f 3.3 ghz 4-core processador cpu de 8 linhas l3 ...</t>
+          <t>núcleo i3-12100f i3 12100f 3.3 ghz 4-core processador cpu de 8 linhas l3 = 12m ...</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>553.04</v>
+        <v>549.92</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005261208077.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECMUK&amp;usg=AOvVaw1csN_JYFa-Djl7vHQALjQI</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005195505536.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECPEK&amp;usg=AOvVaw2JE3XCWlgKnOkMR-7xmMsr</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>placa mãe msi pro h610m-g ddr4 - lga 1700</t>
+          <t>100% novo intel core i3 12100f 3.3 ghz 4-core processador cpu de 8 linhas l3 ...</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>555.09</v>
+        <v>553.04</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://patoloco.com.br/placa-mae-msi-pro-h610m-g-intel-lga-1700-matx-ddr4&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECOcQ&amp;usg=AOvVaw1awuZY4HYN_xFCRY8hbSBA</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005261208077.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECNYK&amp;usg=AOvVaw0iyKCRsNxioVluLmrbwSzq</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>novo intel core i3 12100f 3.3 ghz 4-core processador cpu de 8 linhas l3 = 12m 58w ...</t>
+          <t>placa mãe msi pro h610m-g ddr4 - lga 1700</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>557.87</v>
+        <v>555.09</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005221677129.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECOoJ&amp;usg=AOvVaw2LuEOzapNhhCILUaVtzOlB</t>
+          <t>https://www.google.com.br/url?url=https://patoloco.com.br/placa-mae-msi-pro-h610m-g-intel-lga-1700-matx-ddr4&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECMwQ&amp;usg=AOvVaw29ZCd9Flnt_Q0eapKZ8nWm</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>placa mãe asus prime h610m-a d4 lga 1700 h610 matx ddr4</t>
+          <t>novo intel core i3 12100f 3.3 ghz 4-core processador cpu de 8 linhas l3 = 12m 58w ...</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>557.99</v>
+        <v>557.87</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.tradeinn.com/techinn/pt/asus-placa-mae-prime-h610m-a-d4/138689539/p%3Futm_source%3Dgoogle_products%26utm_medium%3Dmerchant%26id_producte%3D15514222%26country%3Dbr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECPcN&amp;usg=AOvVaw2VDXGZXziOxHEQlMOKBrm8</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005221677129.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECPsJ&amp;usg=AOvVaw2WJqSiUlj3AQ7_W4oW6PnL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>placa mãe asus prime h610m-a d4 (csm) lga 1700 ddr4</t>
+          <t>placa mãe asus prime h610m-a d4 lga 1700 h610 matx ddr4</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>575.99</v>
+        <v>557.99</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.tradeinn.com/techinn/pt/asus-placa-mae-prime-h610m-a-d4-csm/138689540/p%3Futm_source%3Dgoogle_products%26utm_medium%3Dmerchant%26id_producte%3D15514223%26country%3Dbr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECNgT&amp;usg=AOvVaw3xcTkIWtm2unDaFP6Eo4Sh</t>
+          <t>https://www.google.com.br/url?url=https://www.tradeinn.com/techinn/pt/asus-placa-mae-prime-h610m-a-d4/138689539/p%3Futm_source%3Dgoogle_products%26utm_medium%3Dmerchant%26id_producte%3D15514222%26country%3Dbr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECOsN&amp;usg=AOvVaw3PyTKiH9Gtf9dkrlZgJYBA</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pichau.com.br/placa-mae-biostar-h610mx-e-ddr4-socket-lga1700-m-atx-chipset-intel-h610-h610mx-e%3Fsrsltid%3DAd5pg_GQPbf7qYUr6Wao9JiRUL3HxRX_-pv3n-qGQXgINCbJq0DgqqURVRk&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECJMO&amp;usg=AOvVaw2wY4vt0Ir3WV0z6C3vtpge</t>
+          <t>https://www.google.com.br/url?url=https://www.pichau.com.br/placa-mae-biostar-h610mx-e-ddr4-socket-lga1700-m-atx-chipset-intel-h610-h610mx-e%3Fsrsltid%3DAd5pg_HJRjcrdD3wrtFOnDt77f2kYg8LgsokobYMHp3RyFMq0pIFhjwD9ys&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECIcO&amp;usg=AOvVaw041675mzSt1LHn6idCEJt7</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004958855375.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECLkK&amp;usg=AOvVaw38WyMJY6uiabiO1N9ukKzn</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004958855375.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECMoK&amp;usg=AOvVaw3XaeViuJbspurP1rm3I4LP</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.concordia.inf.br/placa-mae-gigabyte-h610m-h-ddr4-chipset-h610-intel-lga-1700-matx-ddr4%3Fparceiro%3D2180%26srsltid%3DAd5pg_EfMhTzHjksu0cocOHpPfWvTBquF_-DrN8sRg93_XlbGuhzEUNgZ4k&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECPUT&amp;usg=AOvVaw1aPl6PVw4fxL32FL5G_omE</t>
+          <t>https://www.google.com.br/url?url=https://www.concordia.inf.br/placa-mae-gigabyte-h610m-h-ddr4-chipset-h610-intel-lga-1700-matx-ddr4%3Fparceiro%3D2180%26srsltid%3DAd5pg_HRBtIP0SnFykzOla_Jb6JjBo1i_rqb1imm3pDRMbkDdIZnWsxPlNw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECL0T&amp;usg=AOvVaw28bsXQARrBsMy7m6XLMBIR</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.compulink.com.br/informatica/placa-mae/placa-mae-intel-1700-h610m-m-2-2xddr4-hdmivgadp-12ag-h610m-k-m-2-colorful%3Fparceiro%3D2506%26srsltid%3DAd5pg_HW4_fjijn2HF430NCpxFLJSG2gCoblKTjF9pcY0cJDngOID0Tna8Y&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECNcQ&amp;usg=AOvVaw2QItc7sIuvgWOpqmgWBfDn</t>
+          <t>https://www.google.com.br/url?url=https://www.compulink.com.br/informatica/placa-mae/placa-mae-intel-1700-h610m-m-2-2xddr4-hdmivgadp-12ag-h610m-k-m-2-colorful%3Fparceiro%3D2506%26srsltid%3DAd5pg_F1GBAEy_KlvNWTh1Wu5rz9dOYeIE3lR_BEYgug5lp8_yi_wXmK0FA&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECLwQ&amp;usg=AOvVaw0AVK8evutyP21Z65o2iu1v</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-3307715666-placa-me-asrock-h610m-hvs-chipset-h610-intel-lga-1700-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECPQQ&amp;usg=AOvVaw1cxPLrzDDYPfRelWrq3Rlx</t>
+          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-3307715666-placa-me-asrock-h610m-hvs-chipset-h610-intel-lga-1700-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECOcQ&amp;usg=AOvVaw39DrcSb_ZbY5WbudLO4tOt</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.magazineluiza.com.br/placa-mae-asus-prime-h610m-k-d4-matx-lga-1700-ddr4-hdmi-vga-m-2-usb-3-2-90mb1a10-m0eay0/p/ke7h8g8b1g/in/pmae/%3F%26seller_id%3Dgigantec&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECIUO&amp;usg=AOvVaw3iujzSjpg9pBtO2Hs2oaWl</t>
+          <t>https://www.google.com.br/url?url=https://www.magazineluiza.com.br/placa-mae-asus-prime-h610m-k-d4-matx-lga-1700-ddr4-hdmi-vga-m-2-usb-3-2-90mb1a10-m0eay0/p/ke7h8g8b1g/in/pmae/%3F%26seller_id%3Dgigantec&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECPkN&amp;usg=AOvVaw2qXREIDWCbAad17FxI2ics</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.extra.com.br/placa-mae-mancer-h610m-dawt-ddr4-socket-lga1700-m-atx-chipset-intel-h610-mcr-h610m-dawt-1553923960/p/1553923960%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1553923960%26idLojista%3D40028%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECOIP&amp;usg=AOvVaw064n_P54A_AAauF316NSCl</t>
+          <t>https://www.google.com.br/url?url=https://www.extra.com.br/placa-mae-mancer-h610m-dawt-ddr4-socket-lga1700-m-atx-chipset-intel-h610-mcr-h610m-dawt-1553923960/p/1553923960%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1553923960%26idLojista%3D40028%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECOYP&amp;usg=AOvVaw3mqhTDmPG_--3BggH6ehX8</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-3232227342-placa-mae-msi-pro-h610m-g-ddr4-intel-lga-1700-matx-h610-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECL8S&amp;usg=AOvVaw3VRHPbKisrOvAaNNiZ0QLG</t>
+          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-3232227342-placa-mae-msi-pro-h610m-g-ddr4-intel-lga-1700-matx-h610-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECLIS&amp;usg=AOvVaw2X6k9bThMIHKI2OfJEdaD1</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004891033935.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECNAN&amp;usg=AOvVaw3uDsFx8mEpylkbYInpDSe6</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004891033935.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECOIN&amp;usg=AOvVaw2SPhAF5ktFCQ-YY_eJsmg5</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/placa-mae-mancer-h610m-da-ddr4-socket-lga1700-m-atx-chipset-intel-h610-mcr-h610m-da-1546542279/p/1546542279%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1546542279%26idLojista%3D40028%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECJgP&amp;usg=AOvVaw1VhEC-mQlBfF4P1ctnVQhs</t>
+          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/placa-mae-mancer-h610m-da-ddr4-socket-lga1700-m-atx-chipset-intel-h610-mcr-h610m-da-1546542279/p/1546542279%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1546542279%26idLojista%3D40028%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECIwP&amp;usg=AOvVaw0HWV03G9s29V8Gj9sGYkxZ</t>
         </is>
       </c>
     </row>
@@ -896,7 +896,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/placa-mae-h610-ddr4-m2-10-100-1000-lga1700-hdmi-vga-dpport-1554309357/p/1554309357%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1554309357%26idLojista%3D11121%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECLoT&amp;usg=AOvVaw3KDzpuIlkWOIMvnpUqI8l8</t>
+          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/placa-mae-h610-ddr4-m2-10-100-1000-lga1700-hdmi-vga-dpport-1554309357/p/1554309357%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1554309357%26idLojista%3D11121%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECI8T&amp;usg=AOvVaw2tLjbVeG7IhLBQFLFCE0O6</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/321070/placa-mae-asus-prime-h610m-e-d4-intel-lga-1700-matx-ddr4%3Fsrsltid%3DAd5pg_E9S8fn_Wy6i1rvS2IOrnkBrP4Haqz6ZTlRi7W0R7IaV2E1IVGH5l0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECMsN&amp;usg=AOvVaw1vi_3nEFuBWjXAK305hO1w</t>
+          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/321070/placa-mae-asus-prime-h610m-e-d4-intel-lga-1700-matx-ddr4%3Fsrsltid%3DAd5pg_Gn8hrItTlar5a8NvpdJtx7LfCLqH50nBY-08dioaAlcSCZZejPW5k&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECL8N&amp;usg=AOvVaw2yuYMSmFKIvDFNhCIsWiyY</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.tradeinn.com/techinn/pt/gigabyte-placa-mae-h610i/139712323/p%3Futm_source%3Dgoogle_products%26utm_medium%3Dmerchant%26id_producte%3D19201639%26country%3Dbr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECJAR&amp;usg=AOvVaw2zKsOsKWi1_RUO4w3dQbkd</t>
+          <t>https://www.google.com.br/url?url=https://www.tradeinn.com/techinn/pt/gigabyte-placa-mae-h610i/139712323/p%3Futm_source%3Dgoogle_products%26utm_medium%3Dmerchant%26id_producte%3D19201639%26country%3Dbr&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECPUQ&amp;usg=AOvVaw1VOdZLNOGoJ_f3wEwJfpF4</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.hdstore.com.br/processador-intel-core-i3-12100f-33ghz-turbo-43ghz-12mb-cache-lga1700-12-geracao-bx8071512100f%3Fsrsltid%3DAd5pg_FjfFMLQbovS4vV957J-_Lm5uApxke_U1A19NpH_rWwPZjmEu3LAH0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECJkL&amp;usg=AOvVaw36ZlPJzThfT6urMkXi2buB</t>
+          <t>https://www.google.com.br/url?url=https://www.hdstore.com.br/processador-intel-core-i3-12100f-33ghz-turbo-43ghz-12mb-cache-lga1700-12-geracao-bx8071512100f%3Fsrsltid%3DAd5pg_FgshSmbUrnxqgC7tk6ahKOzCDT46gTx1YzYW8PUNACegBV1gc4E9M&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECKoL&amp;usg=AOvVaw3ssCBt_-VS3-qZqWfMKFcU</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.microgem.com.br/hardware/processadores/processador-intel/processador-intel-core-i3-12100f-cache-12mb-3-3ghz-4-3ghz-max-turbo-lga-1700-bx8071512100f&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECJAM&amp;usg=AOvVaw1vgjCVar4X7z70ap7r977C</t>
+          <t>https://www.google.com.br/url?url=https://www.microgem.com.br/hardware/processadores/processador-intel/processador-intel-core-i3-12100f-cache-12mb-3-3ghz-4-3ghz-max-turbo-lga-1700-bx8071512100f&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECKEM&amp;usg=AOvVaw1ALqshRteG27xiEgsvmuOe</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.carrefour.com.br/placa-mae-intel-1700-h610m-2xddr4-hdmiusb-12-geracao-h610mhvs-asrock-mp929508798/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECIEQ&amp;usg=AOvVaw0uLaOoXixeZIZDIMOhtrSb</t>
+          <t>https://www.google.com.br/url?url=https://www.carrefour.com.br/placa-mae-intel-1700-h610m-2xddr4-hdmiusb-12-geracao-h610mhvs-asrock-mp929508798/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECPUP&amp;usg=AOvVaw3QMffhMVGOc5RcZTmOqPCo</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.hardstore.com.br/shop/products/placa-mae-asus-prime-h610m-e-d4-lga-1700-intel-h610-m-2&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECMkT&amp;usg=AOvVaw0SpgAnU4VjSjafqYsgyroS</t>
+          <t>https://www.google.com.br/url?url=https://www.hardstore.com.br/shop/products/placa-mae-asus-prime-h610m-e-d4-lga-1700-intel-h610-m-2&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECK4T&amp;usg=AOvVaw3ybVPg1n0gF7hl_Je_jRct</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://tiendamia.com/br/producto%3Famz%3DB09NPJX7PV&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQguUECPcJ&amp;usg=AOvVaw1D4VGICYpk5W5M1Wv7vrUh</t>
+          <t>https://www.google.com.br/url?url=https://tiendamia.com/br/producto%3Famz%3DB09NPJX7PV&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQguUECIgK&amp;usg=AOvVaw0b6F-uOyksv7zeRAvCUfah</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005002914387.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECKoT&amp;usg=AOvVaw2pcKifAyJSYHWeVrVhLTuE</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005002914387.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECPAS&amp;usg=AOvVaw0atiaKvHZgdbdOP95Lz5AI</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/430125/processador-intel-lga-1200-i3-12100f-s-video-c-cooler-tray%3Fsrsltid%3DAd5pg_FfKrXlMPAkvqx_dZj1E-dATnSdfxoDbgMow8DHW7CxmCuMB5Lh1zQ&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQguUECIQK&amp;usg=AOvVaw2nyS567W9eyIpbN-n3mN5M</t>
+          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/430125/processador-intel-lga-1200-i3-12100f-s-video-c-cooler-tray%3Fsrsltid%3DAd5pg_H17NtXl5WcGiPwgWV5307vCfvS6ZZx_icixtZVqlvbQMulTkP_vLs&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQguUECJUK&amp;usg=AOvVaw3dNfcmZG0qOKuklrkAlTQB</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-2893057349-placa-me-gigabyte-h610m-h-ddr4-micro-atx-lga-1700-12-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQguUECNoN&amp;usg=AOvVaw3pI5SJ1faN8SOXDAvBNuGd</t>
+          <t>https://www.google.com.br/url?url=https://produto.mercadolivre.com.br/MLB-2893057349-placa-me-gigabyte-h610m-h-ddr4-micro-atx-lga-1700-12-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQguUECM4N&amp;usg=AOvVaw0q_QLdO74gRmGdh0SiWyo3</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005093287462.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiy2O-zkvX9AhWmq5UCHRpdA0IQgOUECKMS&amp;usg=AOvVaw1PbGQiBUcvVEt2wIJ88YAL</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005093287462.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjv0MaEmfX9AhW4pZUCHZ43DowQgOUECJYS&amp;usg=AOvVaw0U5z0raHs_B4AfBblAvEEw</t>
         </is>
       </c>
     </row>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/processador-intel-core-i3-12100f-330ghz-12mb-lga-1700-12-ger-bx8071512100f-1532138510/p/1532138510%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1532138510%26idLojista%3D112169%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECNsM&amp;usg=AOvVaw3uy6DaiC3FW4_EB7AjlhBj</t>
+          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/processador-intel-core-i3-12100f-330ghz-12mb-lga-1700-12-ger-bx8071512100f-1532138510/p/1532138510%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1532138510%26idLojista%3D112169%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECPcM&amp;usg=AOvVaw1JdA9yJokOSNptsraNWjr9</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.studiopc.com.br/processador-intel-core-i3-12100f-33ghz-43ghz-turbo-12-geracao-4-cores-8-threads-lga-1700-bx8071512100f&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECI0O&amp;usg=AOvVaw3z672mEk5ADHEhdrpB9JRl</t>
+          <t>https://www.google.com.br/url?url=https://www.studiopc.com.br/processador-intel-core-i3-12100f-33ghz-43ghz-turbo-12-geracao-4-cores-8-threads-lga-1700-bx8071512100f&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECLkO&amp;usg=AOvVaw2lpL2ViFN10utcVW5b4My7</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/422662/processador-intel-core-i3-12100f-3-30ghz-lga-1700%3Fsrsltid%3DAd5pg_EMHFIITyBqPeva8nGG42YhrYzqI8jiFN79699IPK7kpump3hNO-ds&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQguUECNAJ&amp;usg=AOvVaw2jKobgDf-asntrejpC4rxq</t>
+          <t>https://www.google.com.br/url?url=https://www.kabum.com.br/produto/422662/processador-intel-core-i3-12100f-3-30ghz-lga-1700%3Fsrsltid%3DAd5pg_GOWzxnwOctZuoZqcL3cSWvxEJEcpsVGYPoniJH--0KOccqdIRtI7o&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQguUECOEJ&amp;usg=AOvVaw1tEipC6HrgW6ZYNbhxAQJ6</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.casasbahia.com.br/processador-intel-core-i3-12100f-4-core-8-threads-33ghz-43ghz-turbo-cache-12mb-lga1700-bx8071512100f-1547567861/p/1547567861%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1547567861%26idLojista%3D164340%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECKUP&amp;usg=AOvVaw1s2ZM226SxUo4suaFuIGI0</t>
+          <t>https://www.google.com.br/url?url=https://www.casasbahia.com.br/processador-intel-core-i3-12100f-4-core-8-threads-33ghz-43ghz-turbo-cache-12mb-lga1700-bx8071512100f-1547567861/p/1547567861%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1547567861%26idLojista%3D164340%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECLQP&amp;usg=AOvVaw3r9_SUGrdzGpBV2RA0lpqI</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004024703577.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECLQL&amp;usg=AOvVaw35b35YgWZIAL4Bg5leQWYA</t>
+          <t>https://www.google.com.br/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004024703577.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECMUL&amp;usg=AOvVaw09S87u6Wvhto1gQ-oD3tm7</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/processador-intel-core-i3-12100f-33ghz-43ghz-turbo-lga1700-12mb-cache-12-ger-bx8071512100f-1540299894/p/1540299894%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1540299894%26idLojista%3D13600%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECPYL&amp;usg=AOvVaw3kcj_d6Y6-NYsH6IyH45h9</t>
+          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/processador-intel-core-i3-12100f-33ghz-43ghz-turbo-lga1700-12mb-cache-12-ger-bx8071512100f-1540299894/p/1540299894%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1540299894%26idLojista%3D13600%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECIcM&amp;usg=AOvVaw0tu9BANDhFzSauaE8fhGoG</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://gamernareal.com.br/product/processador-intel-core-i3-12100f/%3Futm_source%3DGoogle%2520Shopping%26utm_campaign%3DGoogle%2520Menor%2520Preco%26utm_medium%3Dcpc%26utm_term%3D5840&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECOQO&amp;usg=AOvVaw3wpdMp1-p1I2WOz-qZnHMe</t>
+          <t>https://www.google.com.br/url?url=https://gamernareal.com.br/product/processador-intel-core-i3-12100f/%3Futm_source%3DGoogle%2520Shopping%26utm_campaign%3DGoogle%2520Menor%2520Preco%26utm_medium%3Dcpc%26utm_term%3D5840&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECPUO&amp;usg=AOvVaw3P7aNUeuTUAnPttbFuV4l2</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.chipware.com.br/proc-intel-core-i3-12100f-s1700-330ghz-12mb-grafico-nao-integrado-box-com-cooler%3Fsrsltid%3DAd5pg_G9bkL3EOfClQbvt0F44BRMALoqHUS0c-hKde8tnQhQGKDCv9nK3OM&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECIwN&amp;usg=AOvVaw1AGkTPWc5pmL3e8kOuZ-R8</t>
+          <t>https://www.google.com.br/url?url=https://www.chipware.com.br/proc-intel-core-i3-12100f-s1700-330ghz-12mb-grafico-nao-integrado-box-com-cooler%3Fsrsltid%3DAd5pg_HISPbeATb7HtyFZl5fJzkC2Quzon0AHhn-69G-y9XxtlL8LfkfUr4&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECJ0N&amp;usg=AOvVaw1buYpKBC2L5Cm7_dGCvoNC</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.americanas.com.br/produto/5421126584%3Fopn%3DYSMESP%26offerId%3D62ce8fca4862ecc395eaa519%26srsltid%3DAd5pg_HPT61ubJaIHFiRTvNnjMHyMUvVYhE-Z91mQBRBtmZUl4_XaPbP6FY&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECOYM&amp;usg=AOvVaw1oKAwrlJBaa0bJSBFFFt5a</t>
+          <t>https://www.google.com.br/url?url=https://www.americanas.com.br/produto/5421126584%3Fopn%3DYSMESP%26offerId%3D62ce8fca4862ecc395eaa519%26srsltid%3DAd5pg_Ge-ytZzFxJ1lAkijTzmDY1U17e8dHGddaSqoNO2pi4pMaNjyscxhU&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECOsM&amp;usg=AOvVaw0BDbJJXzbB-RAkZL04IwoH</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.casasbahia.com.br/processador-intel-core-i3-12100f-33ghz-43ghz-turbo-1553614482/p/1553614482%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1553614482%26idLojista%3D11121%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECIAN&amp;usg=AOvVaw0jdahqtdyK_NlP2KxG20Ue</t>
+          <t>https://www.google.com.br/url?url=https://www.casasbahia.com.br/processador-intel-core-i3-12100f-33ghz-43ghz-turbo-1553614482/p/1553614482%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1553614482%26idLojista%3D11121%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECIMN&amp;usg=AOvVaw1S2mcdDBNHYXalVFSfcGOA</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.extra.com.br/processador-intel-core-i3-12100f-330ghz-lga-1700-12-ger-1549963400/p/1549963400%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1549963400%26idLojista%3D145305%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECN4L&amp;usg=AOvVaw3Khi5CAe3lEyEQCNchKac4</t>
+          <t>https://www.google.com.br/url?url=https://www.extra.com.br/processador-intel-core-i3-12100f-330ghz-lga-1700-12-ger-1549963400/p/1549963400%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1549963400%26idLojista%3D145305%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECO8L&amp;usg=AOvVaw14itZ70S_OZ4b55eBbcy-v</t>
         </is>
       </c>
     </row>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.eletti.com.br/hardware/processador/processador-intel-core-i3-12100f-p1700&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECIEO&amp;usg=AOvVaw0UZoaiXlFFkX_ULA2FgIxh</t>
+          <t>https://www.google.com.br/url?url=https://www.eletti.com.br/hardware/processador/processador-intel-core-i3-12100f-p1700&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECK0O&amp;usg=AOvVaw3SW9uy3XInG6HCX2KNUjUk</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.carrefour.com.br/processador-intel-core-i312100f-lga1700-33ghz-bx8071512100f-mp931736707/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECKYO&amp;usg=AOvVaw2dODHBMDSpMSUUIg9ab103</t>
+          <t>https://www.google.com.br/url?url=https://www.carrefour.com.br/processador-intel-core-i312100f-lga1700-33ghz-bx8071512100f-mp931736707/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECNIO&amp;usg=AOvVaw1wyfVr7tq7-RxnntObwJi7</t>
         </is>
       </c>
     </row>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://arenacomputadores.com/produto/processador-intel-i3-12100f/%3Fsrsltid%3DAd5pg_GfwOvrm0Nh2yhBeua7S-6s4UJJ9BMdiS055hvjwsT3GgkJwhYIxS0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECMQN&amp;usg=AOvVaw1m1DKWb3aL3fNpxODw7Mtp</t>
+          <t>https://www.google.com.br/url?url=https://arenacomputadores.com/produto/processador-intel-i3-12100f/%3Fsrsltid%3DAd5pg_F2x69bybImDBLchjNGwoeribbZTp2AOQGzE38_o8Uwl1cT630Hz_A&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECO8N&amp;usg=AOvVaw1diKThJSKyD4t0sePaYLq4</t>
         </is>
       </c>
     </row>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/processador-intel-core-i3-12100f-lga1700-33-ghz-4-cores-e-8-threads-bx8071512100f-1555122913/p/1555122913%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1555122913%26idLojista%3D141877%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiCi_aukvX9AhXqpZUCHRabDOIQgOUECPAO&amp;usg=AOvVaw0_TNt7JxK4T-e5mWOxFVnd</t>
+          <t>https://www.google.com.br/url?url=https://www.pontofrio.com.br/processador-intel-core-i3-12100f-lga1700-33-ghz-4-cores-e-8-threads-bx8071512100f-1555122913/p/1555122913%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1555122913%26idLojista%3D141877%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjys7P_mPX9AhUgppUCHbQjCLQQgOUECIEP&amp;usg=AOvVaw3JoNE0kwY7FweLaepC1-Tw</t>
         </is>
       </c>
     </row>

</xml_diff>